<commit_message>
Comments and explanatory notes
</commit_message>
<xml_diff>
--- a/LoanAmortiser.xlsx
+++ b/LoanAmortiser.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pauls\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pauls\OneDrive\Documents\Projects\qa-engineer-challenge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66502BE9-D1FC-40E3-B0E8-FC61B87D9D82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{900D5607-54E7-47F2-975E-4641ADE4D62B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -592,7 +592,7 @@
   <dimension ref="A2:K311"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,7 +623,7 @@
       </c>
       <c r="K3" s="6">
         <f>B9</f>
-        <v>1349.9877795487257</v>
+        <v>1305.4198569601867</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -631,11 +631,11 @@
         <v>2</v>
       </c>
       <c r="B4" s="11">
-        <v>7.5</v>
+        <v>4.2</v>
       </c>
       <c r="C4" s="4">
         <f>B4/100/12</f>
-        <v>6.2499999999999995E-3</v>
+        <v>3.5000000000000001E-3</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
@@ -645,7 +645,7 @@
       </c>
       <c r="K4" s="8">
         <f>K5-B3</f>
-        <v>2399.7067091694262</v>
+        <v>1330.0765670444816</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -660,7 +660,7 @@
       </c>
       <c r="K5" s="10">
         <f>SUM(B9:B308)</f>
-        <v>32399.706709169426</v>
+        <v>31330.076567044482</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -689,7 +689,7 @@
       </c>
       <c r="B9" s="1">
         <f>IF(A9&gt;B$5,0,B$3*C$4*(1+C$4)^B$5)/((1+C$4)^B$5-1)</f>
-        <v>1349.9877795487257</v>
+        <v>1305.4198569601867</v>
       </c>
       <c r="C9" s="1">
         <f>B3</f>
@@ -702,11 +702,11 @@
       </c>
       <c r="B10" s="1">
         <f t="shared" ref="B10:B73" si="0">IF(A10&gt;B$5,0,B$3*C$4*(1+C$4)^B$5)/((1+C$4)^B$5-1)</f>
-        <v>1349.9877795487257</v>
+        <v>1305.4198569601867</v>
       </c>
       <c r="C10" s="1">
         <f>(C9*(1+C$4))-B9</f>
-        <v>28837.512220451277</v>
+        <v>28799.580143039813</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -715,11 +715,11 @@
       </c>
       <c r="B11" s="1">
         <f t="shared" si="0"/>
-        <v>1349.9877795487257</v>
+        <v>1305.4198569601867</v>
       </c>
       <c r="C11" s="1">
         <f t="shared" ref="C11:C74" si="1">(C10*(1+C$4))-B10</f>
-        <v>27667.758892280373</v>
+        <v>27594.958816580267</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -728,11 +728,11 @@
       </c>
       <c r="B12" s="1">
         <f t="shared" si="0"/>
-        <v>1349.9877795487257</v>
+        <v>1305.4198569601867</v>
       </c>
       <c r="C12" s="1">
         <f t="shared" si="1"/>
-        <v>26490.694605808403</v>
+        <v>26386.121315478114</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -741,11 +741,11 @@
       </c>
       <c r="B13" s="1">
         <f t="shared" si="0"/>
-        <v>1349.9877795487257</v>
+        <v>1305.4198569601867</v>
       </c>
       <c r="C13" s="1">
         <f t="shared" si="1"/>
-        <v>25306.273667545982</v>
+        <v>25173.052883122102</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -754,11 +754,11 @@
       </c>
       <c r="B14" s="1">
         <f t="shared" si="0"/>
-        <v>1349.9877795487257</v>
+        <v>1305.4198569601867</v>
       </c>
       <c r="C14" s="1">
         <f t="shared" si="1"/>
-        <v>24114.45009841942</v>
+        <v>23955.738711252845</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -767,11 +767,11 @@
       </c>
       <c r="B15" s="1">
         <f t="shared" si="0"/>
-        <v>1349.9877795487257</v>
+        <v>1305.4198569601867</v>
       </c>
       <c r="C15" s="1">
         <f t="shared" si="1"/>
-        <v>22915.177631985818</v>
+        <v>22734.163939782044</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -780,11 +780,11 @@
       </c>
       <c r="B16" s="1">
         <f t="shared" si="0"/>
-        <v>1349.9877795487257</v>
+        <v>1305.4198569601867</v>
       </c>
       <c r="C16" s="1">
         <f t="shared" si="1"/>
-        <v>21708.409712637003</v>
+        <v>21508.313656611095</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -793,11 +793,11 @@
       </c>
       <c r="B17" s="1">
         <f t="shared" si="0"/>
-        <v>1349.9877795487257</v>
+        <v>1305.4198569601867</v>
       </c>
       <c r="C17" s="1">
         <f t="shared" si="1"/>
-        <v>20494.099493792259</v>
+        <v>20278.172897449047</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -806,11 +806,11 @@
       </c>
       <c r="B18" s="1">
         <f t="shared" si="0"/>
-        <v>1349.9877795487257</v>
+        <v>1305.4198569601867</v>
       </c>
       <c r="C18" s="1">
         <f t="shared" si="1"/>
-        <v>19272.199836079737</v>
+        <v>19043.726645629933</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -819,11 +819,11 @@
       </c>
       <c r="B19" s="1">
         <f t="shared" si="0"/>
-        <v>1349.9877795487257</v>
+        <v>1305.4198569601867</v>
       </c>
       <c r="C19" s="1">
         <f t="shared" si="1"/>
-        <v>18042.66330550651</v>
+        <v>17804.959831929453</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -832,11 +832,11 @@
       </c>
       <c r="B20" s="1">
         <f t="shared" si="0"/>
-        <v>1349.9877795487257</v>
+        <v>1305.4198569601867</v>
       </c>
       <c r="C20" s="1">
         <f t="shared" si="1"/>
-        <v>16805.4421716172</v>
+        <v>16561.85733438102</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -845,11 +845,11 @@
       </c>
       <c r="B21" s="1">
         <f t="shared" si="0"/>
-        <v>1349.9877795487257</v>
+        <v>1305.4198569601867</v>
       </c>
       <c r="C21" s="1">
         <f t="shared" si="1"/>
-        <v>15560.488405641081</v>
+        <v>15314.40397809117</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -858,11 +858,11 @@
       </c>
       <c r="B22" s="1">
         <f t="shared" si="0"/>
-        <v>1349.9877795487257</v>
+        <v>1305.4198569601867</v>
       </c>
       <c r="C22" s="1">
         <f t="shared" si="1"/>
-        <v>14307.753678627612</v>
+        <v>14062.584535054302</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -871,11 +871,11 @@
       </c>
       <c r="B23" s="1">
         <f t="shared" si="0"/>
-        <v>1349.9877795487257</v>
+        <v>1305.4198569601867</v>
       </c>
       <c r="C23" s="1">
         <f t="shared" si="1"/>
-        <v>13047.18935957031</v>
+        <v>12806.383723966806</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -884,11 +884,11 @@
       </c>
       <c r="B24" s="1">
         <f t="shared" si="0"/>
-        <v>1349.9877795487257</v>
+        <v>1305.4198569601867</v>
       </c>
       <c r="C24" s="1">
         <f t="shared" si="1"/>
-        <v>11778.7465135189</v>
+        <v>11545.786210040504</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -897,11 +897,11 @@
       </c>
       <c r="B25" s="1">
         <f t="shared" si="0"/>
-        <v>1349.9877795487257</v>
+        <v>1305.4198569601867</v>
       </c>
       <c r="C25" s="1">
         <f t="shared" si="1"/>
-        <v>10502.375899679668</v>
+        <v>10280.776604815459</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -910,11 +910,11 @@
       </c>
       <c r="B26" s="1">
         <f t="shared" si="0"/>
-        <v>1349.9877795487257</v>
+        <v>1305.4198569601867</v>
       </c>
       <c r="C26" s="1">
         <f t="shared" si="1"/>
-        <v>9218.0279695039408</v>
+        <v>9011.3394659721271</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -923,11 +923,11 @@
       </c>
       <c r="B27" s="1">
         <f t="shared" si="0"/>
-        <v>1349.9877795487257</v>
+        <v>1305.4198569601867</v>
       </c>
       <c r="C27" s="1">
         <f t="shared" si="1"/>
-        <v>7925.6528647646164</v>
+        <v>7737.4592971428428</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -936,11 +936,11 @@
       </c>
       <c r="B28" s="1">
         <f t="shared" si="0"/>
-        <v>1349.9877795487257</v>
+        <v>1305.4198569601867</v>
       </c>
       <c r="C28" s="1">
         <f t="shared" si="1"/>
-        <v>6625.2004156206704</v>
+        <v>6459.1205477226567</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -949,11 +949,11 @@
       </c>
       <c r="B29" s="1">
         <f t="shared" si="0"/>
-        <v>1349.9877795487257</v>
+        <v>1305.4198569601867</v>
       </c>
       <c r="C29" s="1">
         <f t="shared" si="1"/>
-        <v>5316.6201386695748</v>
+        <v>5176.3076126794995</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -962,11 +962,11 @@
       </c>
       <c r="B30" s="1">
         <f t="shared" si="0"/>
-        <v>1349.9877795487257</v>
+        <v>1305.4198569601867</v>
       </c>
       <c r="C30" s="1">
         <f t="shared" si="1"/>
-        <v>3999.8612349875348</v>
+        <v>3889.0048323636911</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -975,11 +975,11 @@
       </c>
       <c r="B31" s="1">
         <f t="shared" si="0"/>
-        <v>1349.9877795487257</v>
+        <v>1305.4198569601867</v>
       </c>
       <c r="C31" s="1">
         <f t="shared" si="1"/>
-        <v>2674.8725881574819</v>
+        <v>2597.1964923167775</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -988,11 +988,11 @@
       </c>
       <c r="B32" s="1">
         <f t="shared" si="0"/>
-        <v>1349.9877795487257</v>
+        <v>1305.4198569601867</v>
       </c>
       <c r="C32" s="1">
         <f t="shared" si="1"/>
-        <v>1341.6027622847407</v>
+        <v>1300.8668230796998</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -1005,7 +1005,7 @@
       </c>
       <c r="C33" s="1">
         <f t="shared" si="1"/>
-        <v>2.9467628337442875E-10</v>
+        <v>2.9194779926910996E-10</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -1018,7 +1018,7 @@
       </c>
       <c r="C34" s="1">
         <f t="shared" si="1"/>
-        <v>2.9651801014551896E-10</v>
+        <v>2.9296961656655188E-10</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -1031,7 +1031,7 @@
       </c>
       <c r="C35" s="1">
         <f t="shared" si="1"/>
-        <v>2.983712477089285E-10</v>
+        <v>2.9399501022453484E-10</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -1044,7 +1044,7 @@
       </c>
       <c r="C36" s="1">
         <f t="shared" si="1"/>
-        <v>3.0023606800710933E-10</v>
+        <v>2.9502399276032075E-10</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -1057,7 +1057,7 @@
       </c>
       <c r="C37" s="1">
         <f t="shared" si="1"/>
-        <v>3.0211254343215377E-10</v>
+        <v>2.9605657673498187E-10</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -1070,7 +1070,7 @@
       </c>
       <c r="C38" s="1">
         <f t="shared" si="1"/>
-        <v>3.0400074682860475E-10</v>
+        <v>2.9709277475355432E-10</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -1083,7 +1083,7 @@
       </c>
       <c r="C39" s="1">
         <f t="shared" si="1"/>
-        <v>3.0590075149628358E-10</v>
+        <v>2.9813259946519179E-10</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -1096,7 +1096,7 @@
       </c>
       <c r="C40" s="1">
         <f t="shared" si="1"/>
-        <v>3.0781263119313537E-10</v>
+        <v>2.9917606356331998E-10</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -1109,7 +1109,7 @@
       </c>
       <c r="C41" s="1">
         <f t="shared" si="1"/>
-        <v>3.0973646013809248E-10</v>
+        <v>3.0022317978579163E-10</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -1122,7 +1122,7 @@
       </c>
       <c r="C42" s="1">
         <f t="shared" si="1"/>
-        <v>3.1167231301395558E-10</v>
+        <v>3.0127396091504192E-10</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -1135,7 +1135,7 @@
       </c>
       <c r="C43" s="1">
         <f t="shared" si="1"/>
-        <v>3.1362026497029283E-10</v>
+        <v>3.0232841977824458E-10</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -1148,7 +1148,7 @@
       </c>
       <c r="C44" s="1">
         <f t="shared" si="1"/>
-        <v>3.1558039162635717E-10</v>
+        <v>3.0338656924746845E-10</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -1161,7 +1161,7 @@
       </c>
       <c r="C45" s="1">
         <f t="shared" si="1"/>
-        <v>3.1755276907402191E-10</v>
+        <v>3.0444842223983461E-10</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -1174,7 +1174,7 @@
       </c>
       <c r="C46" s="1">
         <f t="shared" si="1"/>
-        <v>3.1953747388073456E-10</v>
+        <v>3.0551399171767405E-10</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -1187,7 +1187,7 @@
       </c>
       <c r="C47" s="1">
         <f t="shared" si="1"/>
-        <v>3.2153458309248917E-10</v>
+        <v>3.0658329068868593E-10</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -1200,7 +1200,7 @@
       </c>
       <c r="C48" s="1">
         <f t="shared" si="1"/>
-        <v>3.2354417423681725E-10</v>
+        <v>3.0765633220609637E-10</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -1213,7 +1213,7 @@
       </c>
       <c r="C49" s="1">
         <f t="shared" si="1"/>
-        <v>3.255663253257974E-10</v>
+        <v>3.0873312936881773E-10</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -1226,7 +1226,7 @@
       </c>
       <c r="C50" s="1">
         <f t="shared" si="1"/>
-        <v>3.2760111485908367E-10</v>
+        <v>3.0981369532160861E-10</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -1239,7 +1239,7 @@
       </c>
       <c r="C51" s="1">
         <f t="shared" si="1"/>
-        <v>3.2964862182695298E-10</v>
+        <v>3.1089804325523425E-10</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -1252,7 +1252,7 @@
       </c>
       <c r="C52" s="1">
         <f t="shared" si="1"/>
-        <v>3.3170892571337147E-10</v>
+        <v>3.119861864066276E-10</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -1265,7 +1265,7 @@
       </c>
       <c r="C53" s="1">
         <f t="shared" si="1"/>
-        <v>3.3378210649908007E-10</v>
+        <v>3.1307813805905084E-10</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -1278,7 +1278,7 @@
       </c>
       <c r="C54" s="1">
         <f t="shared" si="1"/>
-        <v>3.3586824466469933E-10</v>
+        <v>3.1417391154225753E-10</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -1291,7 +1291,7 @@
       </c>
       <c r="C55" s="1">
         <f t="shared" si="1"/>
-        <v>3.3796742119385371E-10</v>
+        <v>3.1527352023265546E-10</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -1304,7 +1304,7 @@
       </c>
       <c r="C56" s="1">
         <f t="shared" si="1"/>
-        <v>3.4007971757631533E-10</v>
+        <v>3.1637697755346976E-10</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -1317,7 +1317,7 @@
       </c>
       <c r="C57" s="1">
         <f t="shared" si="1"/>
-        <v>3.4220521581116731E-10</v>
+        <v>3.1748429697490692E-10</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -1330,7 +1330,7 @@
       </c>
       <c r="C58" s="1">
         <f t="shared" si="1"/>
-        <v>3.4434399840998712E-10</v>
+        <v>3.1859549201431914E-10</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -1343,7 +1343,7 @@
       </c>
       <c r="C59" s="1">
         <f t="shared" si="1"/>
-        <v>3.4649614840004958E-10</v>
+        <v>3.1971057623636929E-10</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -1356,7 +1356,7 @@
       </c>
       <c r="C60" s="1">
         <f t="shared" si="1"/>
-        <v>3.4866174932754993E-10</v>
+        <v>3.2082956325319658E-10</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -1369,7 +1369,7 @@
       </c>
       <c r="C61" s="1">
         <f t="shared" si="1"/>
-        <v>3.5084088526084713E-10</v>
+        <v>3.2195246672458279E-10</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -1382,7 +1382,7 @@
       </c>
       <c r="C62" s="1">
         <f t="shared" si="1"/>
-        <v>3.5303364079372747E-10</v>
+        <v>3.2307930035811887E-10</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -1395,7 +1395,7 @@
       </c>
       <c r="C63" s="1">
         <f t="shared" si="1"/>
-        <v>3.552401010486883E-10</v>
+        <v>3.242100779093723E-10</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -1408,7 +1408,7 @@
       </c>
       <c r="C64" s="1">
         <f t="shared" si="1"/>
-        <v>3.5746035168024265E-10</v>
+        <v>3.253448131820551E-10</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -1421,7 +1421,7 @@
       </c>
       <c r="C65" s="1">
         <f t="shared" si="1"/>
-        <v>3.5969447887824422E-10</v>
+        <v>3.2648352002819229E-10</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -1434,7 +1434,7 @@
       </c>
       <c r="C66" s="1">
         <f t="shared" si="1"/>
-        <v>3.6194256937123325E-10</v>
+        <v>3.2762621234829096E-10</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -1447,7 +1447,7 @@
       </c>
       <c r="C67" s="1">
         <f t="shared" si="1"/>
-        <v>3.642047104298035E-10</v>
+        <v>3.2877290409150997E-10</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -1460,7 +1460,7 @@
       </c>
       <c r="C68" s="1">
         <f t="shared" si="1"/>
-        <v>3.6648098986998983E-10</v>
+        <v>3.2992360925583026E-10</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -1473,7 +1473,7 @@
       </c>
       <c r="C69" s="1">
         <f t="shared" si="1"/>
-        <v>3.6877149605667727E-10</v>
+        <v>3.3107834188822566E-10</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -1486,7 +1486,7 @@
       </c>
       <c r="C70" s="1">
         <f t="shared" si="1"/>
-        <v>3.7107631790703155E-10</v>
+        <v>3.3223711608483445E-10</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -1499,7 +1499,7 @@
       </c>
       <c r="C71" s="1">
         <f t="shared" si="1"/>
-        <v>3.7339554489395051E-10</v>
+        <v>3.333999459911314E-10</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -1512,7 +1512,7 @@
       </c>
       <c r="C72" s="1">
         <f t="shared" si="1"/>
-        <v>3.7572926704953775E-10</v>
+        <v>3.3456684580210036E-10</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -1525,7 +1525,7 @@
       </c>
       <c r="C73" s="1">
         <f t="shared" si="1"/>
-        <v>3.7807757496859738E-10</v>
+        <v>3.3573782976240775E-10</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -1538,7 +1538,7 @@
       </c>
       <c r="C74" s="1">
         <f t="shared" si="1"/>
-        <v>3.8044055981215115E-10</v>
+        <v>3.3691291216657619E-10</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -1551,7 +1551,7 @@
       </c>
       <c r="C75" s="1">
         <f t="shared" ref="C75:C138" si="3">(C74*(1+C$4))-B74</f>
-        <v>3.8281831331097713E-10</v>
+        <v>3.3809210735915921E-10</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -1564,7 +1564,7 @@
       </c>
       <c r="C76" s="1">
         <f t="shared" si="3"/>
-        <v>3.8521092776917078E-10</v>
+        <v>3.3927542973491627E-10</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -1577,7 +1577,7 @@
       </c>
       <c r="C77" s="1">
         <f t="shared" si="3"/>
-        <v>3.8761849606772811E-10</v>
+        <v>3.4046289373898849E-10</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -1590,7 +1590,7 @@
       </c>
       <c r="C78" s="1">
         <f t="shared" si="3"/>
-        <v>3.9004111166815142E-10</v>
+        <v>3.4165451386707498E-10</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -1603,7 +1603,7 @@
       </c>
       <c r="C79" s="1">
         <f t="shared" si="3"/>
-        <v>3.9247886861607742E-10</v>
+        <v>3.4285030466560978E-10</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -1616,7 +1616,7 @@
       </c>
       <c r="C80" s="1">
         <f t="shared" si="3"/>
-        <v>3.9493186154492793E-10</v>
+        <v>3.4405028073193942E-10</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -1629,7 +1629,7 @@
       </c>
       <c r="C81" s="1">
         <f t="shared" si="3"/>
-        <v>3.9740018567958377E-10</v>
+        <v>3.4525445671450125E-10</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -1642,7 +1642,7 @@
       </c>
       <c r="C82" s="1">
         <f t="shared" si="3"/>
-        <v>3.9988393684008118E-10</v>
+        <v>3.4646284731300205E-10</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
@@ -1655,7 +1655,7 @@
       </c>
       <c r="C83" s="1">
         <f t="shared" si="3"/>
-        <v>4.0238321144533174E-10</v>
+        <v>3.4767546727859757E-10</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -1668,7 +1668,7 @@
       </c>
       <c r="C84" s="1">
         <f t="shared" si="3"/>
-        <v>4.048981065168651E-10</v>
+        <v>3.4889233141407266E-10</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -1681,7 +1681,7 @@
       </c>
       <c r="C85" s="1">
         <f t="shared" si="3"/>
-        <v>4.0742871968259554E-10</v>
+        <v>3.5011345457402192E-10</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -1694,7 +1694,7 @@
       </c>
       <c r="C86" s="1">
         <f t="shared" si="3"/>
-        <v>4.0997514918061181E-10</v>
+        <v>3.5133885166503102E-10</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -1707,7 +1707,7 @@
       </c>
       <c r="C87" s="1">
         <f t="shared" si="3"/>
-        <v>4.1253749386299068E-10</v>
+        <v>3.5256853764585867E-10</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -1720,7 +1720,7 @@
       </c>
       <c r="C88" s="1">
         <f t="shared" si="3"/>
-        <v>4.1511585319963442E-10</v>
+        <v>3.538025275276192E-10</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -1733,7 +1733,7 @@
       </c>
       <c r="C89" s="1">
         <f t="shared" si="3"/>
-        <v>4.1771032728213216E-10</v>
+        <v>3.5504083637396586E-10</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -1746,7 +1746,7 @@
       </c>
       <c r="C90" s="1">
         <f t="shared" si="3"/>
-        <v>4.2032101682764551E-10</v>
+        <v>3.5628347930127477E-10</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -1759,7 +1759,7 @@
       </c>
       <c r="C91" s="1">
         <f t="shared" si="3"/>
-        <v>4.2294802318281831E-10</v>
+        <v>3.5753047147882924E-10</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -1772,7 +1772,7 @@
       </c>
       <c r="C92" s="1">
         <f t="shared" si="3"/>
-        <v>4.2559144832771095E-10</v>
+        <v>3.5878182812900515E-10</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -1785,7 +1785,7 @@
       </c>
       <c r="C93" s="1">
         <f t="shared" si="3"/>
-        <v>4.2825139487975917E-10</v>
+        <v>3.6003756452745668E-10</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -1798,7 +1798,7 @@
       </c>
       <c r="C94" s="1">
         <f t="shared" si="3"/>
-        <v>4.3092796609775771E-10</v>
+        <v>3.6129769600330277E-10</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -1811,7 +1811,7 @@
       </c>
       <c r="C95" s="1">
         <f t="shared" si="3"/>
-        <v>4.3362126588586871E-10</v>
+        <v>3.6256223793931436E-10</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -1824,7 +1824,7 @@
       </c>
       <c r="C96" s="1">
         <f t="shared" si="3"/>
-        <v>4.3633139879765541E-10</v>
+        <v>3.6383120577210198E-10</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -1837,7 +1837,7 @@
       </c>
       <c r="C97" s="1">
         <f t="shared" si="3"/>
-        <v>4.3905847004014079E-10</v>
+        <v>3.6510461499230437E-10</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -1850,7 +1850,7 @@
       </c>
       <c r="C98" s="1">
         <f t="shared" si="3"/>
-        <v>4.4180258547789171E-10</v>
+        <v>3.6638248114477745E-10</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
@@ -1863,7 +1863,7 @@
       </c>
       <c r="C99" s="1">
         <f t="shared" si="3"/>
-        <v>4.4456385163712857E-10</v>
+        <v>3.6766481982878418E-10</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
@@ -1876,7 +1876,7 @@
       </c>
       <c r="C100" s="1">
         <f t="shared" si="3"/>
-        <v>4.4734237570986067E-10</v>
+        <v>3.6895164669818493E-10</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
@@ -1889,7 +1889,7 @@
       </c>
       <c r="C101" s="1">
         <f t="shared" si="3"/>
-        <v>4.5013826555804735E-10</v>
+        <v>3.7024297746162863E-10</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
@@ -1902,7 +1902,7 @@
       </c>
       <c r="C102" s="1">
         <f t="shared" si="3"/>
-        <v>4.529516297177852E-10</v>
+        <v>3.7153882788274437E-10</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
@@ -1915,7 +1915,7 @@
       </c>
       <c r="C103" s="1">
         <f t="shared" si="3"/>
-        <v>4.5578257740352138E-10</v>
+        <v>3.7283921378033402E-10</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
@@ -1928,7 +1928,7 @@
       </c>
       <c r="C104" s="1">
         <f t="shared" si="3"/>
-        <v>4.5863121851229344E-10</v>
+        <v>3.7414415102856522E-10</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
@@ -1941,7 +1941,7 @@
       </c>
       <c r="C105" s="1">
         <f t="shared" si="3"/>
-        <v>4.6149766362799532E-10</v>
+        <v>3.7545365555716521E-10</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
@@ -1954,7 +1954,7 @@
       </c>
       <c r="C106" s="1">
         <f t="shared" si="3"/>
-        <v>4.6438202402567034E-10</v>
+        <v>3.7676774335161533E-10</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
@@ -1967,7 +1967,7 @@
       </c>
       <c r="C107" s="1">
         <f t="shared" si="3"/>
-        <v>4.6728441167583087E-10</v>
+        <v>3.7808643045334601E-10</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
@@ -1980,7 +1980,7 @@
       </c>
       <c r="C108" s="1">
         <f t="shared" si="3"/>
-        <v>4.7020493924880489E-10</v>
+        <v>3.7940973295993272E-10</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
@@ -1993,7 +1993,7 @@
       </c>
       <c r="C109" s="1">
         <f t="shared" si="3"/>
-        <v>4.7314372011910998E-10</v>
+        <v>3.8073766702529249E-10</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
@@ -2006,7 +2006,7 @@
       </c>
       <c r="C110" s="1">
         <f t="shared" si="3"/>
-        <v>4.7610086836985448E-10</v>
+        <v>3.8207024885988102E-10</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
@@ -2019,7 +2019,7 @@
       </c>
       <c r="C111" s="1">
         <f t="shared" si="3"/>
-        <v>4.7907649879716615E-10</v>
+        <v>3.8340749473089062E-10</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
@@ -2032,7 +2032,7 @@
       </c>
       <c r="C112" s="1">
         <f t="shared" si="3"/>
-        <v>4.8207072691464849E-10</v>
+        <v>3.8474942096244878E-10</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
@@ -2045,7 +2045,7 @@
       </c>
       <c r="C113" s="1">
         <f t="shared" si="3"/>
-        <v>4.8508366895786509E-10</v>
+        <v>3.8609604393581736E-10</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
@@ -2058,7 +2058,7 @@
       </c>
       <c r="C114" s="1">
         <f t="shared" si="3"/>
-        <v>4.8811544188885175E-10</v>
+        <v>3.8744738008959276E-10</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
@@ -2071,7 +2071,7 @@
       </c>
       <c r="C115" s="1">
         <f t="shared" si="3"/>
-        <v>4.9116616340065709E-10</v>
+        <v>3.8880344591990635E-10</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
@@ -2084,7 +2084,7 @@
       </c>
       <c r="C116" s="1">
         <f t="shared" si="3"/>
-        <v>4.9423595192191124E-10</v>
+        <v>3.9016425798062602E-10</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
@@ -2097,7 +2097,7 @@
       </c>
       <c r="C117" s="1">
         <f t="shared" si="3"/>
-        <v>4.9732492662142322E-10</v>
+        <v>3.9152983288355824E-10</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
@@ -2110,7 +2110,7 @@
       </c>
       <c r="C118" s="1">
         <f t="shared" si="3"/>
-        <v>5.0043320741280717E-10</v>
+        <v>3.9290018729865071E-10</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
@@ -2123,7 +2123,7 @@
       </c>
       <c r="C119" s="1">
         <f t="shared" si="3"/>
-        <v>5.0356091495913729E-10</v>
+        <v>3.94275337954196E-10</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
@@ -2136,7 +2136,7 @@
       </c>
       <c r="C120" s="1">
         <f t="shared" si="3"/>
-        <v>5.0670817067763196E-10</v>
+        <v>3.9565530163703573E-10</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
@@ -2149,7 +2149,7 @@
       </c>
       <c r="C121" s="1">
         <f t="shared" si="3"/>
-        <v>5.0987509674436723E-10</v>
+        <v>3.9704009519276536E-10</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
@@ -2162,7 +2162,7 @@
       </c>
       <c r="C122" s="1">
         <f t="shared" si="3"/>
-        <v>5.1306181609901957E-10</v>
+        <v>3.9842973552594004E-10</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
@@ -2175,7 +2175,7 @@
       </c>
       <c r="C123" s="1">
         <f t="shared" si="3"/>
-        <v>5.1626845244963845E-10</v>
+        <v>3.9982423960028088E-10</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
@@ -2188,7 +2188,7 @@
       </c>
       <c r="C124" s="1">
         <f t="shared" si="3"/>
-        <v>5.1949513027744872E-10</v>
+        <v>4.0122362443888188E-10</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
@@ -2201,7 +2201,7 @@
       </c>
       <c r="C125" s="1">
         <f t="shared" si="3"/>
-        <v>5.2274197484168281E-10</v>
+        <v>4.0262790712441799E-10</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
@@ -2214,7 +2214,7 @@
       </c>
       <c r="C126" s="1">
         <f t="shared" si="3"/>
-        <v>5.2600911218444337E-10</v>
+        <v>4.040371047993535E-10</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
@@ -2227,7 +2227,7 @@
       </c>
       <c r="C127" s="1">
         <f t="shared" si="3"/>
-        <v>5.2929666913559623E-10</v>
+        <v>4.0545123466615125E-10</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
@@ -2240,7 +2240,7 @@
       </c>
       <c r="C128" s="1">
         <f t="shared" si="3"/>
-        <v>5.3260477331769379E-10</v>
+        <v>4.0687031398748282E-10</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
@@ -2253,7 +2253,7 @@
       </c>
       <c r="C129" s="1">
         <f t="shared" si="3"/>
-        <v>5.359335531509294E-10</v>
+        <v>4.0829436008643901E-10</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
@@ -2266,7 +2266,7 @@
       </c>
       <c r="C130" s="1">
         <f t="shared" si="3"/>
-        <v>5.3928313785812277E-10</v>
+        <v>4.0972339034674156E-10</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
@@ -2279,7 +2279,7 @@
       </c>
       <c r="C131" s="1">
         <f t="shared" si="3"/>
-        <v>5.4265365746973604E-10</v>
+        <v>4.111574222129552E-10</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
@@ -2292,7 +2292,7 @@
       </c>
       <c r="C132" s="1">
         <f t="shared" si="3"/>
-        <v>5.460452428289219E-10</v>
+        <v>4.1259647319070057E-10</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
@@ -2305,7 +2305,7 @@
       </c>
       <c r="C133" s="1">
         <f t="shared" si="3"/>
-        <v>5.4945802559660275E-10</v>
+        <v>4.1404056084686804E-10</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
@@ -2318,7 +2318,7 @@
       </c>
       <c r="C134" s="1">
         <f t="shared" si="3"/>
-        <v>5.5289213825658157E-10</v>
+        <v>4.1548970280983213E-10</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
@@ -2331,7 +2331,7 @@
       </c>
       <c r="C135" s="1">
         <f t="shared" si="3"/>
-        <v>5.563477141206853E-10</v>
+        <v>4.1694391676966656E-10</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
@@ -2344,7 +2344,7 @@
       </c>
       <c r="C136" s="1">
         <f t="shared" si="3"/>
-        <v>5.5982488733393961E-10</v>
+        <v>4.184032204783604E-10</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
@@ -2357,7 +2357,7 @@
       </c>
       <c r="C137" s="1">
         <f t="shared" si="3"/>
-        <v>5.6332379287977678E-10</v>
+        <v>4.198676317500347E-10</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
@@ -2370,7 +2370,7 @@
       </c>
       <c r="C138" s="1">
         <f t="shared" si="3"/>
-        <v>5.6684456658527546E-10</v>
+        <v>4.2133716846115984E-10</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
@@ -2383,7 +2383,7 @@
       </c>
       <c r="C139" s="1">
         <f t="shared" ref="C139:C202" si="5">(C138*(1+C$4))-B138</f>
-        <v>5.7038734512643352E-10</v>
+        <v>4.2281184855077391E-10</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
@@ -2396,7 +2396,7 @@
       </c>
       <c r="C140" s="1">
         <f t="shared" si="5"/>
-        <v>5.739522660334738E-10</v>
+        <v>4.2429169002070166E-10</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
@@ -2409,7 +2409,7 @@
       </c>
       <c r="C141" s="1">
         <f t="shared" si="5"/>
-        <v>5.7753946769618306E-10</v>
+        <v>4.2577671093577415E-10</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
@@ -2422,7 +2422,7 @@
       </c>
       <c r="C142" s="1">
         <f t="shared" si="5"/>
-        <v>5.8114908936928428E-10</v>
+        <v>4.2726692942404938E-10</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
@@ -2435,7 +2435,7 @@
       </c>
       <c r="C143" s="1">
         <f t="shared" si="5"/>
-        <v>5.8478127117784232E-10</v>
+        <v>4.2876236367703356E-10</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
@@ -2448,7 +2448,7 @@
       </c>
       <c r="C144" s="1">
         <f t="shared" si="5"/>
-        <v>5.8843615412270384E-10</v>
+        <v>4.3026303194990322E-10</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
@@ -2461,7 +2461,7 @@
       </c>
       <c r="C145" s="1">
         <f t="shared" si="5"/>
-        <v>5.921138800859708E-10</v>
+        <v>4.3176895256172793E-10</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
@@ -2474,7 +2474,7 @@
       </c>
       <c r="C146" s="1">
         <f t="shared" si="5"/>
-        <v>5.9581459183650816E-10</v>
+        <v>4.3328014389569398E-10</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
@@ -2487,7 +2487,7 @@
       </c>
       <c r="C147" s="1">
         <f t="shared" si="5"/>
-        <v>5.9953843303548641E-10</v>
+        <v>4.3479662439932894E-10</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
@@ -2500,7 +2500,7 @@
       </c>
       <c r="C148" s="1">
         <f t="shared" si="5"/>
-        <v>6.0328554824195822E-10</v>
+        <v>4.3631841258472662E-10</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
@@ -2513,7 +2513,7 @@
       </c>
       <c r="C149" s="1">
         <f t="shared" si="5"/>
-        <v>6.0705608291847051E-10</v>
+        <v>4.3784552702877317E-10</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
@@ -2526,7 +2526,7 @@
       </c>
       <c r="C150" s="1">
         <f t="shared" si="5"/>
-        <v>6.1085018343671096E-10</v>
+        <v>4.3937798637337392E-10</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
@@ -2539,7 +2539,7 @@
       </c>
       <c r="C151" s="1">
         <f t="shared" si="5"/>
-        <v>6.1466799708319044E-10</v>
+        <v>4.4091580932568077E-10</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
@@ -2552,7 +2552,7 @@
       </c>
       <c r="C152" s="1">
         <f t="shared" si="5"/>
-        <v>6.1850967206496039E-10</v>
+        <v>4.4245901465832069E-10</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
@@ -2565,7 +2565,7 @@
       </c>
       <c r="C153" s="1">
         <f t="shared" si="5"/>
-        <v>6.2237535751536646E-10</v>
+        <v>4.4400762120962482E-10</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
@@ -2578,7 +2578,7 @@
       </c>
       <c r="C154" s="1">
         <f t="shared" si="5"/>
-        <v>6.2626520349983754E-10</v>
+        <v>4.4556164788385855E-10</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
@@ -2591,7 +2591,7 @@
       </c>
       <c r="C155" s="1">
         <f t="shared" si="5"/>
-        <v>6.3017936102171161E-10</v>
+        <v>4.4712111365145206E-10</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
@@ -2604,7 +2604,7 @@
       </c>
       <c r="C156" s="1">
         <f t="shared" si="5"/>
-        <v>6.3411798202809732E-10</v>
+        <v>4.4868603754923214E-10</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
@@ -2617,7 +2617,7 @@
       </c>
       <c r="C157" s="1">
         <f t="shared" si="5"/>
-        <v>6.3808121941577297E-10</v>
+        <v>4.5025643868065449E-10</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
@@ -2630,7 +2630,7 @@
       </c>
       <c r="C158" s="1">
         <f t="shared" si="5"/>
-        <v>6.4206922703712158E-10</v>
+        <v>4.5183233621603681E-10</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
@@ -2643,7 +2643,7 @@
       </c>
       <c r="C159" s="1">
         <f t="shared" si="5"/>
-        <v>6.4608215970610367E-10</v>
+        <v>4.5341374939279297E-10</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
@@ -2656,7 +2656,7 @@
       </c>
       <c r="C160" s="1">
         <f t="shared" si="5"/>
-        <v>6.5012017320426687E-10</v>
+        <v>4.5500069751566777E-10</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
@@ -2669,7 +2669,7 @@
       </c>
       <c r="C161" s="1">
         <f t="shared" si="5"/>
-        <v>6.5418342428679357E-10</v>
+        <v>4.5659319995697261E-10</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
@@ -2682,7 +2682,7 @@
       </c>
       <c r="C162" s="1">
         <f t="shared" si="5"/>
-        <v>6.5827207068858605E-10</v>
+        <v>4.5819127615682205E-10</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
@@ -2695,7 +2695,7 @@
       </c>
       <c r="C163" s="1">
         <f t="shared" si="5"/>
-        <v>6.6238627113038972E-10</v>
+        <v>4.5979494562337094E-10</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
@@ -2708,7 +2708,7 @@
       </c>
       <c r="C164" s="1">
         <f t="shared" si="5"/>
-        <v>6.6652618532495474E-10</v>
+        <v>4.6140422793305277E-10</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
@@ -2721,7 +2721,7 @@
       </c>
       <c r="C165" s="1">
         <f t="shared" si="5"/>
-        <v>6.7069197398323579E-10</v>
+        <v>4.6301914273081847E-10</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
@@ -2734,7 +2734,7 @@
       </c>
       <c r="C166" s="1">
         <f t="shared" si="5"/>
-        <v>6.7488379882063103E-10</v>
+        <v>4.6463970973037635E-10</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
@@ -2747,7 +2747,7 @@
       </c>
       <c r="C167" s="1">
         <f t="shared" si="5"/>
-        <v>6.7910182256326005E-10</v>
+        <v>4.6626594871443274E-10</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
@@ -2760,7 +2760,7 @@
       </c>
       <c r="C168" s="1">
         <f t="shared" si="5"/>
-        <v>6.8334620895428044E-10</v>
+        <v>4.6789787953493329E-10</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
@@ -2773,7 +2773,7 @@
       </c>
       <c r="C169" s="1">
         <f t="shared" si="5"/>
-        <v>6.8761712276024478E-10</v>
+        <v>4.6953552211330555E-10</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
@@ -2786,7 +2786,7 @@
       </c>
       <c r="C170" s="1">
         <f t="shared" si="5"/>
-        <v>6.919147297774964E-10</v>
+        <v>4.7117889644070219E-10</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
@@ -2799,7 +2799,7 @@
       </c>
       <c r="C171" s="1">
         <f t="shared" si="5"/>
-        <v>6.9623919683860578E-10</v>
+        <v>4.7282802257824471E-10</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
@@ -2812,7 +2812,7 @@
       </c>
       <c r="C172" s="1">
         <f t="shared" si="5"/>
-        <v>7.0059069181884715E-10</v>
+        <v>4.7448292065726859E-10</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
@@ -2825,7 +2825,7 @@
       </c>
       <c r="C173" s="1">
         <f t="shared" si="5"/>
-        <v>7.0496938364271505E-10</v>
+        <v>4.7614361087956909E-10</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
@@ -2838,7 +2838,7 @@
       </c>
       <c r="C174" s="1">
         <f t="shared" si="5"/>
-        <v>7.0937544229048208E-10</v>
+        <v>4.7781011351764759E-10</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
@@ -2851,7 +2851,7 @@
       </c>
       <c r="C175" s="1">
         <f t="shared" si="5"/>
-        <v>7.1380903880479764E-10</v>
+        <v>4.7948244891495942E-10</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
@@ -2864,7 +2864,7 @@
       </c>
       <c r="C176" s="1">
         <f t="shared" si="5"/>
-        <v>7.1827034529732772E-10</v>
+        <v>4.811606374861618E-10</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
@@ -2877,7 +2877,7 @@
       </c>
       <c r="C177" s="1">
         <f t="shared" si="5"/>
-        <v>7.2275953495543605E-10</v>
+        <v>4.8284469971736335E-10</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
@@ -2890,7 +2890,7 @@
       </c>
       <c r="C178" s="1">
         <f t="shared" si="5"/>
-        <v>7.2727678204890758E-10</v>
+        <v>4.8453465616637412E-10</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
@@ -2903,7 +2903,7 @@
       </c>
       <c r="C179" s="1">
         <f t="shared" si="5"/>
-        <v>7.3182226193671333E-10</v>
+        <v>4.8623052746295648E-10</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
@@ -2916,7 +2916,7 @@
       </c>
       <c r="C180" s="1">
         <f t="shared" si="5"/>
-        <v>7.3639615107381782E-10</v>
+        <v>4.8793233430907687E-10</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
@@ -2929,7 +2929,7 @@
       </c>
       <c r="C181" s="1">
         <f t="shared" si="5"/>
-        <v>7.4099862701802922E-10</v>
+        <v>4.8964009747915872E-10</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
@@ -2942,7 +2942,7 @@
       </c>
       <c r="C182" s="1">
         <f t="shared" si="5"/>
-        <v>7.4562986843689197E-10</v>
+        <v>4.9135383782033577E-10</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
@@ -2955,7 +2955,7 @@
       </c>
       <c r="C183" s="1">
         <f t="shared" si="5"/>
-        <v>7.5029005511462266E-10</v>
+        <v>4.9307357625270697E-10</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
@@ -2968,7 +2968,7 @@
       </c>
       <c r="C184" s="1">
         <f t="shared" si="5"/>
-        <v>7.549793679590891E-10</v>
+        <v>4.9479933376959151E-10</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
@@ -2981,7 +2981,7 @@
       </c>
       <c r="C185" s="1">
         <f t="shared" si="5"/>
-        <v>7.5969798900883343E-10</v>
+        <v>4.9653113143778508E-10</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
@@ -2994,7 +2994,7 @@
       </c>
       <c r="C186" s="1">
         <f t="shared" si="5"/>
-        <v>7.6444610144013869E-10</v>
+        <v>4.9826899039781734E-10</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
@@ -3007,7 +3007,7 @@
       </c>
       <c r="C187" s="1">
         <f t="shared" si="5"/>
-        <v>7.6922388957413962E-10</v>
+        <v>5.0001293186420975E-10</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
@@ -3020,7 +3020,7 @@
       </c>
       <c r="C188" s="1">
         <f t="shared" si="5"/>
-        <v>7.7403153888397805E-10</v>
+        <v>5.0176297712573449E-10</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
@@ -3033,7 +3033,7 @@
       </c>
       <c r="C189" s="1">
         <f t="shared" si="5"/>
-        <v>7.7886923600200298E-10</v>
+        <v>5.0351914754567455E-10</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
@@ -3046,7 +3046,7 @@
       </c>
       <c r="C190" s="1">
         <f t="shared" si="5"/>
-        <v>7.837371687270156E-10</v>
+        <v>5.0528146456208443E-10</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
@@ -3059,7 +3059,7 @@
       </c>
       <c r="C191" s="1">
         <f t="shared" si="5"/>
-        <v>7.8863552603155947E-10</v>
+        <v>5.0704994968805179E-10</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
@@ -3072,7 +3072,7 @@
       </c>
       <c r="C192" s="1">
         <f t="shared" si="5"/>
-        <v>7.9356449806925683E-10</v>
+        <v>5.0882462451195996E-10</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
@@ -3085,7 +3085,7 @@
       </c>
       <c r="C193" s="1">
         <f t="shared" si="5"/>
-        <v>7.9852427618218975E-10</v>
+        <v>5.1060551069775188E-10</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
@@ -3098,7 +3098,7 @@
       </c>
       <c r="C194" s="1">
         <f t="shared" si="5"/>
-        <v>8.0351505290832847E-10</v>
+        <v>5.1239262998519404E-10</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
@@ -3111,7 +3111,7 @@
       </c>
       <c r="C195" s="1">
         <f t="shared" si="5"/>
-        <v>8.0853702198900556E-10</v>
+        <v>5.1418600419014225E-10</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
@@ -3124,7 +3124,7 @@
       </c>
       <c r="C196" s="1">
         <f t="shared" si="5"/>
-        <v>8.135903783764369E-10</v>
+        <v>5.1598565520480783E-10</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
@@ -3137,7 +3137,7 @@
       </c>
       <c r="C197" s="1">
         <f t="shared" si="5"/>
-        <v>8.1867531824128968E-10</v>
+        <v>5.1779160499802463E-10</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
@@ -3150,7 +3150,7 @@
       </c>
       <c r="C198" s="1">
         <f t="shared" si="5"/>
-        <v>8.2379203898029785E-10</v>
+        <v>5.1960387561551775E-10</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
@@ -3163,7 +3163,7 @@
       </c>
       <c r="C199" s="1">
         <f t="shared" si="5"/>
-        <v>8.289407392239248E-10</v>
+        <v>5.2142248918017206E-10</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
@@ -3176,7 +3176,7 @@
       </c>
       <c r="C200" s="1">
         <f t="shared" si="5"/>
-        <v>8.3412161884407443E-10</v>
+        <v>5.2324746789230268E-10</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
@@ -3189,7 +3189,7 @@
       </c>
       <c r="C201" s="1">
         <f t="shared" si="5"/>
-        <v>8.3933487896184993E-10</v>
+        <v>5.2507883402992579E-10</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
@@ -3202,7 +3202,7 @@
       </c>
       <c r="C202" s="1">
         <f t="shared" si="5"/>
-        <v>8.445807219553616E-10</v>
+        <v>5.2691660994903055E-10</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
@@ -3215,7 +3215,7 @@
       </c>
       <c r="C203" s="1">
         <f t="shared" ref="C203:C266" si="7">(C202*(1+C$4))-B202</f>
-        <v>8.498593514675827E-10</v>
+        <v>5.2876081808385222E-10</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
@@ -3228,7 +3228,7 @@
       </c>
       <c r="C204" s="1">
         <f t="shared" si="7"/>
-        <v>8.5517097241425518E-10</v>
+        <v>5.3061148094714576E-10</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
@@ -3241,7 +3241,7 @@
       </c>
       <c r="C205" s="1">
         <f t="shared" si="7"/>
-        <v>8.6051579099184436E-10</v>
+        <v>5.3246862113046078E-10</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
@@ -3254,7 +3254,7 @@
       </c>
       <c r="C206" s="1">
         <f t="shared" si="7"/>
-        <v>8.6589401468554346E-10</v>
+        <v>5.3433226130441739E-10</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
@@ -3267,7 +3267,7 @@
       </c>
       <c r="C207" s="1">
         <f t="shared" si="7"/>
-        <v>8.7130585227732819E-10</v>
+        <v>5.3620242421898291E-10</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
@@ -3280,7 +3280,7 @@
       </c>
       <c r="C208" s="1">
         <f t="shared" si="7"/>
-        <v>8.7675151385406154E-10</v>
+        <v>5.3807913270374935E-10</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
@@ -3293,7 +3293,7 @@
       </c>
       <c r="C209" s="1">
         <f t="shared" si="7"/>
-        <v>8.8223121081564948E-10</v>
+        <v>5.3996240966821253E-10</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
@@ -3306,7 +3306,7 @@
       </c>
       <c r="C210" s="1">
         <f t="shared" si="7"/>
-        <v>8.8774515588324742E-10</v>
+        <v>5.4185227810205132E-10</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
@@ -3319,7 +3319,7 @@
       </c>
       <c r="C211" s="1">
         <f t="shared" si="7"/>
-        <v>8.9329356310751776E-10</v>
+        <v>5.4374876107540848E-10</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
@@ -3332,7 +3332,7 @@
       </c>
       <c r="C212" s="1">
         <f t="shared" si="7"/>
-        <v>8.988766478769398E-10</v>
+        <v>5.4565188173917244E-10</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
@@ -3345,7 +3345,7 @@
       </c>
       <c r="C213" s="1">
         <f t="shared" si="7"/>
-        <v>9.0449462692617078E-10</v>
+        <v>5.4756166332525962E-10</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
@@ -3358,7 +3358,7 @@
       </c>
       <c r="C214" s="1">
         <f t="shared" si="7"/>
-        <v>9.101477183444594E-10</v>
+        <v>5.4947812914689802E-10</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
@@ -3371,7 +3371,7 @@
       </c>
       <c r="C215" s="1">
         <f t="shared" si="7"/>
-        <v>9.1583614158411238E-10</v>
+        <v>5.5140130259891223E-10</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
@@ -3384,7 +3384,7 @@
       </c>
       <c r="C216" s="1">
         <f t="shared" si="7"/>
-        <v>9.2156011746901312E-10</v>
+        <v>5.5333120715800842E-10</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.25">
@@ -3397,7 +3397,7 @@
       </c>
       <c r="C217" s="1">
         <f t="shared" si="7"/>
-        <v>9.2731986820319455E-10</v>
+        <v>5.5526786638306148E-10</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.25">
@@ -3410,7 +3410,7 @@
       </c>
       <c r="C218" s="1">
         <f t="shared" si="7"/>
-        <v>9.3311561737946464E-10</v>
+        <v>5.5721130391540223E-10</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.25">
@@ -3423,7 +3423,7 @@
       </c>
       <c r="C219" s="1">
         <f t="shared" si="7"/>
-        <v>9.3894758998808629E-10</v>
+        <v>5.5916154347910614E-10</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.25">
@@ -3436,7 +3436,7 @@
       </c>
       <c r="C220" s="1">
         <f t="shared" si="7"/>
-        <v>9.4481601242551199E-10</v>
+        <v>5.6111860888128303E-10</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.25">
@@ -3449,7 +3449,7 @@
       </c>
       <c r="C221" s="1">
         <f t="shared" si="7"/>
-        <v>9.5072111250317156E-10</v>
+        <v>5.6308252401236751E-10</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.25">
@@ -3462,7 +3462,7 @@
       </c>
       <c r="C222" s="1">
         <f t="shared" si="7"/>
-        <v>9.5666311945631644E-10</v>
+        <v>5.6505331284641078E-10</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.25">
@@ -3475,7 +3475,7 @@
       </c>
       <c r="C223" s="1">
         <f t="shared" si="7"/>
-        <v>9.6264226395291855E-10</v>
+        <v>5.6703099944137325E-10</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.25">
@@ -3488,7 +3488,7 @@
       </c>
       <c r="C224" s="1">
         <f t="shared" si="7"/>
-        <v>9.6865877810262447E-10</v>
+        <v>5.6901560793941808E-10</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
@@ -3501,7 +3501,7 @@
       </c>
       <c r="C225" s="1">
         <f t="shared" si="7"/>
-        <v>9.7471289546576597E-10</v>
+        <v>5.7100716256720605E-10</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
@@ -3514,7 +3514,7 @@
       </c>
       <c r="C226" s="1">
         <f t="shared" si="7"/>
-        <v>9.8080485106242712E-10</v>
+        <v>5.730056876361913E-10</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
@@ -3527,7 +3527,7 @@
       </c>
       <c r="C227" s="1">
         <f t="shared" si="7"/>
-        <v>9.8693488138156745E-10</v>
+        <v>5.7501120754291797E-10</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.25">
@@ -3540,7 +3540,7 @@
       </c>
       <c r="C228" s="1">
         <f t="shared" si="7"/>
-        <v>9.9310322439020225E-10</v>
+        <v>5.7702374676931821E-10</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.25">
@@ -3553,7 +3553,7 @@
       </c>
       <c r="C229" s="1">
         <f t="shared" si="7"/>
-        <v>9.9931011954264114E-10</v>
+        <v>5.7904332988301086E-10</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.25">
@@ -3566,7 +3566,7 @@
       </c>
       <c r="C230" s="1">
         <f t="shared" si="7"/>
-        <v>1.0055558077897826E-9</v>
+        <v>5.8106998153760143E-10</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
@@ -3579,7 +3579,7 @@
       </c>
       <c r="C231" s="1">
         <f t="shared" si="7"/>
-        <v>1.0118405315884688E-9</v>
+        <v>5.8310372647298309E-10</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.25">
@@ -3592,7 +3592,7 @@
       </c>
       <c r="C232" s="1">
         <f t="shared" si="7"/>
-        <v>1.0181645349108969E-9</v>
+        <v>5.8514458951563858E-10</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
@@ -3605,7 +3605,7 @@
       </c>
       <c r="C233" s="1">
         <f t="shared" si="7"/>
-        <v>1.0245280632540901E-9</v>
+        <v>5.871925955789434E-10</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.25">
@@ -3618,7 +3618,7 @@
       </c>
       <c r="C234" s="1">
         <f t="shared" si="7"/>
-        <v>1.0309313636494282E-9</v>
+        <v>5.8924776966346974E-10</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
@@ -3631,7 +3631,7 @@
       </c>
       <c r="C235" s="1">
         <f t="shared" si="7"/>
-        <v>1.0373746846722371E-9</v>
+        <v>5.9131013685729187E-10</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.25">
@@ -3644,7 +3644,7 @@
       </c>
       <c r="C236" s="1">
         <f t="shared" si="7"/>
-        <v>1.0438582764514387E-9</v>
+        <v>5.933797223362924E-10</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.25">
@@ -3657,7 +3657,7 @@
       </c>
       <c r="C237" s="1">
         <f t="shared" si="7"/>
-        <v>1.0503823906792604E-9</v>
+        <v>5.9545655136446944E-10</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.25">
@@ -3670,7 +3670,7 @@
       </c>
       <c r="C238" s="1">
         <f t="shared" si="7"/>
-        <v>1.0569472806210059E-9</v>
+        <v>5.9754064929424514E-10</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.25">
@@ -3683,7 +3683,7 @@
       </c>
       <c r="C239" s="1">
         <f t="shared" si="7"/>
-        <v>1.0635532011248874E-9</v>
+        <v>5.9963204156677501E-10</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.25">
@@ -3696,7 +3696,7 @@
       </c>
       <c r="C240" s="1">
         <f t="shared" si="7"/>
-        <v>1.070200408631918E-9</v>
+        <v>6.0173075371225877E-10</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.25">
@@ -3709,7 +3709,7 @@
       </c>
       <c r="C241" s="1">
         <f t="shared" si="7"/>
-        <v>1.0768891611858676E-9</v>
+        <v>6.038368113502517E-10</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.25">
@@ -3722,7 +3722,7 @@
       </c>
       <c r="C242" s="1">
         <f t="shared" si="7"/>
-        <v>1.0836197184432794E-9</v>
+        <v>6.0595024018997764E-10</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.25">
@@ -3735,7 +3735,7 @@
       </c>
       <c r="C243" s="1">
         <f t="shared" si="7"/>
-        <v>1.09039234168355E-9</v>
+        <v>6.0807106603064258E-10</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.25">
@@ -3748,7 +3748,7 @@
       </c>
       <c r="C244" s="1">
         <f t="shared" si="7"/>
-        <v>1.0972072938190723E-9</v>
+        <v>6.1019931476174983E-10</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.25">
@@ -3761,7 +3761,7 @@
       </c>
       <c r="C245" s="1">
         <f t="shared" si="7"/>
-        <v>1.1040648394054417E-9</v>
+        <v>6.1233501236341598E-10</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.25">
@@ -3774,7 +3774,7 @@
       </c>
       <c r="C246" s="1">
         <f t="shared" si="7"/>
-        <v>1.1109652446517257E-9</v>
+        <v>6.1447818490668794E-10</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.25">
@@ -3787,7 +3787,7 @@
       </c>
       <c r="C247" s="1">
         <f t="shared" si="7"/>
-        <v>1.117908777430799E-9</v>
+        <v>6.1662885855386139E-10</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.25">
@@ -3800,7 +3800,7 @@
       </c>
       <c r="C248" s="1">
         <f t="shared" si="7"/>
-        <v>1.1248957072897415E-9</v>
+        <v>6.1878705955879998E-10</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.25">
@@ -3813,7 +3813,7 @@
       </c>
       <c r="C249" s="1">
         <f t="shared" si="7"/>
-        <v>1.1319263054603025E-9</v>
+        <v>6.2095281426725585E-10</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.25">
@@ -3826,7 +3826,7 @@
       </c>
       <c r="C250" s="1">
         <f t="shared" si="7"/>
-        <v>1.1390008448694294E-9</v>
+        <v>6.231261491171913E-10</v>
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.25">
@@ -3839,7 +3839,7 @@
       </c>
       <c r="C251" s="1">
         <f t="shared" si="7"/>
-        <v>1.1461196001498635E-9</v>
+        <v>6.253070906391015E-10</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.25">
@@ -3852,7 +3852,7 @@
       </c>
       <c r="C252" s="1">
         <f t="shared" si="7"/>
-        <v>1.1532828476508003E-9</v>
+        <v>6.2749566545633836E-10</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.25">
@@ -3865,7 +3865,7 @@
       </c>
       <c r="C253" s="1">
         <f t="shared" si="7"/>
-        <v>1.1604908654486179E-9</v>
+        <v>6.2969190028543553E-10</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.25">
@@ -3878,7 +3878,7 @@
       </c>
       <c r="C254" s="1">
         <f t="shared" si="7"/>
-        <v>1.167743933357672E-9</v>
+        <v>6.3189582193643462E-10</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.25">
@@ -3891,7 +3891,7 @@
       </c>
       <c r="C255" s="1">
         <f t="shared" si="7"/>
-        <v>1.1750423329411575E-9</v>
+        <v>6.3410745731321217E-10</v>
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.25">
@@ -3904,7 +3904,7 @@
       </c>
       <c r="C256" s="1">
         <f t="shared" si="7"/>
-        <v>1.1823863475220398E-9</v>
+        <v>6.3632683341380846E-10</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.25">
@@ -3917,7 +3917,7 @@
       </c>
       <c r="C257" s="1">
         <f t="shared" si="7"/>
-        <v>1.1897762621940526E-9</v>
+        <v>6.385539773307568E-10</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.25">
@@ -3930,7 +3930,7 @@
       </c>
       <c r="C258" s="1">
         <f t="shared" si="7"/>
-        <v>1.1972123638327656E-9</v>
+        <v>6.407889162514145E-10</v>
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.25">
@@ -3943,7 +3943,7 @@
       </c>
       <c r="C259" s="1">
         <f t="shared" si="7"/>
-        <v>1.2046949411067205E-9</v>
+        <v>6.4303167745829446E-10</v>
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.25">
@@ -3956,7 +3956,7 @@
       </c>
       <c r="C260" s="1">
         <f t="shared" si="7"/>
-        <v>1.2122242844886377E-9</v>
+        <v>6.4528228832939857E-10</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.25">
@@ -3969,7 +3969,7 @@
       </c>
       <c r="C261" s="1">
         <f t="shared" si="7"/>
-        <v>1.2198006862666918E-9</v>
+        <v>6.4754077633855148E-10</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.25">
@@ -3982,7 +3982,7 @@
       </c>
       <c r="C262" s="1">
         <f t="shared" si="7"/>
-        <v>1.2274244405558588E-9</v>
+        <v>6.4980716905573648E-10</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.25">
@@ -3995,7 +3995,7 @@
       </c>
       <c r="C263" s="1">
         <f t="shared" si="7"/>
-        <v>1.235095843309333E-9</v>
+        <v>6.5208149414743159E-10</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.25">
@@ -4008,7 +4008,7 @@
       </c>
       <c r="C264" s="1">
         <f t="shared" si="7"/>
-        <v>1.2428151923300163E-9</v>
+        <v>6.5436377937694759E-10</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.25">
@@ -4021,7 +4021,7 @@
       </c>
       <c r="C265" s="1">
         <f t="shared" si="7"/>
-        <v>1.250582787282079E-9</v>
+        <v>6.5665405260476699E-10</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.25">
@@ -4034,7 +4034,7 @@
       </c>
       <c r="C266" s="1">
         <f t="shared" si="7"/>
-        <v>1.2583989297025921E-9</v>
+        <v>6.5895234178888371E-10</v>
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.25">
@@ -4047,7 +4047,7 @@
       </c>
       <c r="C267" s="1">
         <f t="shared" ref="C267:C309" si="9">(C266*(1+C$4))-B266</f>
-        <v>1.2662639230132333E-9</v>
+        <v>6.6125867498514481E-10</v>
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.25">
@@ -4060,7 +4060,7 @@
       </c>
       <c r="C268" s="1">
         <f t="shared" si="9"/>
-        <v>1.2741780725320662E-9</v>
+        <v>6.6357308034759286E-10</v>
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.25">
@@ -4073,7 +4073,7 @@
       </c>
       <c r="C269" s="1">
         <f t="shared" si="9"/>
-        <v>1.2821416854853917E-9</v>
+        <v>6.6589558612880946E-10</v>
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.25">
@@ -4086,7 +4086,7 @@
       </c>
       <c r="C270" s="1">
         <f t="shared" si="9"/>
-        <v>1.2901550710196754E-9</v>
+        <v>6.682262206802603E-10</v>
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.25">
@@ -4099,7 +4099,7 @@
       </c>
       <c r="C271" s="1">
         <f t="shared" si="9"/>
-        <v>1.2982185402135485E-9</v>
+        <v>6.7056501245264128E-10</v>
       </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.25">
@@ -4112,7 +4112,7 @@
       </c>
       <c r="C272" s="1">
         <f t="shared" si="9"/>
-        <v>1.3063324060898833E-9</v>
+        <v>6.7291198999622555E-10</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.25">
@@ -4125,7 +4125,7 @@
       </c>
       <c r="C273" s="1">
         <f t="shared" si="9"/>
-        <v>1.3144969836279453E-9</v>
+        <v>6.7526718196121239E-10</v>
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.25">
@@ -4138,7 +4138,7 @@
       </c>
       <c r="C274" s="1">
         <f t="shared" si="9"/>
-        <v>1.3227125897756201E-9</v>
+        <v>6.7763061709807664E-10</v>
       </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.25">
@@ -4151,7 +4151,7 @@
       </c>
       <c r="C275" s="1">
         <f t="shared" si="9"/>
-        <v>1.3309795434617179E-9</v>
+        <v>6.8000232425791998E-10</v>
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.25">
@@ -4164,7 +4164,7 @@
       </c>
       <c r="C276" s="1">
         <f t="shared" si="9"/>
-        <v>1.3392981656083538E-9</v>
+        <v>6.823823323928227E-10</v>
       </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.25">
@@ -4177,7 +4177,7 @@
       </c>
       <c r="C277" s="1">
         <f t="shared" si="9"/>
-        <v>1.3476687791434062E-9</v>
+        <v>6.8477067055619758E-10</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.25">
@@ -4190,7 +4190,7 @@
       </c>
       <c r="C278" s="1">
         <f t="shared" si="9"/>
-        <v>1.3560917090130525E-9</v>
+        <v>6.8716736790314428E-10</v>
       </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.25">
@@ -4203,7 +4203,7 @@
       </c>
       <c r="C279" s="1">
         <f t="shared" si="9"/>
-        <v>1.3645672821943843E-9</v>
+        <v>6.8957245369080533E-10</v>
       </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.25">
@@ -4216,7 +4216,7 @@
       </c>
       <c r="C280" s="1">
         <f t="shared" si="9"/>
-        <v>1.3730958277080992E-9</v>
+        <v>6.9198595727872323E-10</v>
       </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.25">
@@ -4229,7 +4229,7 @@
       </c>
       <c r="C281" s="1">
         <f t="shared" si="9"/>
-        <v>1.381677676631275E-9</v>
+        <v>6.9440790812919878E-10</v>
       </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.25">
@@ -4242,7 +4242,7 @@
       </c>
       <c r="C282" s="1">
         <f t="shared" si="9"/>
-        <v>1.3903131621102206E-9</v>
+        <v>6.9683833580765106E-10</v>
       </c>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.25">
@@ -4255,7 +4255,7 @@
       </c>
       <c r="C283" s="1">
         <f t="shared" si="9"/>
-        <v>1.3990026193734096E-9</v>
+        <v>6.9927726998297789E-10</v>
       </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.25">
@@ -4268,7 +4268,7 @@
       </c>
       <c r="C284" s="1">
         <f t="shared" si="9"/>
-        <v>1.4077463857444935E-9</v>
+        <v>7.0172474042791837E-10</v>
       </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.25">
@@ -4281,7 +4281,7 @@
       </c>
       <c r="C285" s="1">
         <f t="shared" si="9"/>
-        <v>1.4165448006553967E-9</v>
+        <v>7.0418077701941617E-10</v>
       </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.25">
@@ -4294,7 +4294,7 @@
       </c>
       <c r="C286" s="1">
         <f t="shared" si="9"/>
-        <v>1.4253982056594931E-9</v>
+        <v>7.0664540973898415E-10</v>
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.25">
@@ -4307,7 +4307,7 @@
       </c>
       <c r="C287" s="1">
         <f t="shared" si="9"/>
-        <v>1.4343069444448652E-9</v>
+        <v>7.0911866867307067E-10</v>
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.25">
@@ -4320,7 +4320,7 @@
       </c>
       <c r="C288" s="1">
         <f t="shared" si="9"/>
-        <v>1.4432713628476458E-9</v>
+        <v>7.1160058401342646E-10</v>
       </c>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.25">
@@ -4333,7 +4333,7 @@
       </c>
       <c r="C289" s="1">
         <f t="shared" si="9"/>
-        <v>1.4522918088654436E-9</v>
+        <v>7.1409118605747345E-10</v>
       </c>
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.25">
@@ -4346,7 +4346,7 @@
       </c>
       <c r="C290" s="1">
         <f t="shared" si="9"/>
-        <v>1.4613686326708527E-9</v>
+        <v>7.1659050520867469E-10</v>
       </c>
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.25">
@@ -4359,7 +4359,7 @@
       </c>
       <c r="C291" s="1">
         <f t="shared" si="9"/>
-        <v>1.4705021866250457E-9</v>
+        <v>7.1909857197690507E-10</v>
       </c>
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.25">
@@ -4372,7 +4372,7 @@
       </c>
       <c r="C292" s="1">
         <f t="shared" si="9"/>
-        <v>1.4796928252914523E-9</v>
+        <v>7.2161541697882425E-10</v>
       </c>
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.25">
@@ -4385,7 +4385,7 @@
       </c>
       <c r="C293" s="1">
         <f t="shared" si="9"/>
-        <v>1.4889409054495241E-9</v>
+        <v>7.2414107093825014E-10</v>
       </c>
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.25">
@@ -4398,7 +4398,7 @@
       </c>
       <c r="C294" s="1">
         <f t="shared" si="9"/>
-        <v>1.4982467861085837E-9</v>
+        <v>7.2667556468653402E-10</v>
       </c>
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.25">
@@ -4411,7 +4411,7 @@
       </c>
       <c r="C295" s="1">
         <f t="shared" si="9"/>
-        <v>1.5076108285217624E-9</v>
+        <v>7.2921892916293694E-10</v>
       </c>
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.25">
@@ -4424,7 +4424,7 @@
       </c>
       <c r="C296" s="1">
         <f t="shared" si="9"/>
-        <v>1.5170333962000236E-9</v>
+        <v>7.3177119541500726E-10</v>
       </c>
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.25">
@@ -4437,7 +4437,7 @@
       </c>
       <c r="C297" s="1">
         <f t="shared" si="9"/>
-        <v>1.526514854926274E-9</v>
+        <v>7.3433239459895979E-10</v>
       </c>
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.25">
@@ -4450,7 +4450,7 @@
       </c>
       <c r="C298" s="1">
         <f t="shared" si="9"/>
-        <v>1.5360555727695633E-9</v>
+        <v>7.3690255798005621E-10</v>
       </c>
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.25">
@@ -4463,7 +4463,7 @@
       </c>
       <c r="C299" s="1">
         <f t="shared" si="9"/>
-        <v>1.5456559200993732E-9</v>
+        <v>7.3948171693298647E-10</v>
       </c>
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.25">
@@ -4476,7 +4476,7 @@
       </c>
       <c r="C300" s="1">
         <f t="shared" si="9"/>
-        <v>1.5553162695999944E-9</v>
+        <v>7.4206990294225194E-10</v>
       </c>
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.25">
@@ -4489,7 +4489,7 @@
       </c>
       <c r="C301" s="1">
         <f t="shared" si="9"/>
-        <v>1.5650369962849944E-9</v>
+        <v>7.4466714760254986E-10</v>
       </c>
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.25">
@@ -4502,7 +4502,7 @@
       </c>
       <c r="C302" s="1">
         <f t="shared" si="9"/>
-        <v>1.5748184775117758E-9</v>
+        <v>7.4727348261915878E-10</v>
       </c>
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.25">
@@ -4515,7 +4515,7 @@
       </c>
       <c r="C303" s="1">
         <f t="shared" si="9"/>
-        <v>1.5846610929962245E-9</v>
+        <v>7.4988893980832583E-10</v>
       </c>
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.25">
@@ -4528,7 +4528,7 @@
       </c>
       <c r="C304" s="1">
         <f t="shared" si="9"/>
-        <v>1.5945652248274511E-9</v>
+        <v>7.5251355109765504E-10</v>
       </c>
     </row>
     <row r="305" spans="1:3" x14ac:dyDescent="0.25">
@@ -4541,7 +4541,7 @@
       </c>
       <c r="C305" s="1">
         <f t="shared" si="9"/>
-        <v>1.6045312574826227E-9</v>
+        <v>7.5514734852649686E-10</v>
       </c>
     </row>
     <row r="306" spans="1:3" x14ac:dyDescent="0.25">
@@ -4554,7 +4554,7 @@
       </c>
       <c r="C306" s="1">
         <f t="shared" si="9"/>
-        <v>1.6145595778418891E-9</v>
+        <v>7.5779036424633961E-10</v>
       </c>
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.25">
@@ -4567,7 +4567,7 @@
       </c>
       <c r="C307" s="1">
         <f t="shared" si="9"/>
-        <v>1.6246505752034012E-9</v>
+        <v>7.604426305212019E-10</v>
       </c>
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.25">
@@ -4580,7 +4580,7 @@
       </c>
       <c r="C308" s="1">
         <f t="shared" si="9"/>
-        <v>1.6348046412984225E-9</v>
+        <v>7.6310417972802611E-10</v>
       </c>
     </row>
     <row r="309" spans="1:3" x14ac:dyDescent="0.25">
@@ -4593,7 +4593,7 @@
       </c>
       <c r="C309" s="3">
         <f t="shared" si="9"/>
-        <v>1.6450221703065378E-9</v>
+        <v>7.6577504435707425E-10</v>
       </c>
     </row>
     <row r="311" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>